<commit_message>
Add width to Data-screening_2021.R, started script to find the difference between cover in 2012 and 2021
</commit_message>
<xml_diff>
--- a/data/Excel_raw/Channel-width_LiDAR-GIS.xlsx
+++ b/data/Excel_raw/Channel-width_LiDAR-GIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_email_arizona_edu/Documents/grad school/Gornish lab/Altar Valley Conservation Alliance Elkhorn-Las Delicias Demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_email_arizona_edu/Documents/grad school/Gornish lab/Altar Valley Conservation Alliance Elkhorn-Las Delicias Demo/AVCA_ElkLD/data/Excel_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="698" documentId="8_{0F1C1F85-34D5-468B-AF89-FA8959926033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD82F825-1E34-463B-9B7B-CFF6CA5D1C75}"/>
+  <xr:revisionPtr revIDLastSave="728" documentId="8_{0F1C1F85-34D5-468B-AF89-FA8959926033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3363BAE6-2DB2-4CF1-9E2D-78F6465C8E5F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{A46D63DB-7B3E-4708-B87A-D559BFA7A94D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A46D63DB-7B3E-4708-B87A-D559BFA7A94D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,194 +125,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Channel</t>
   </si>
   <si>
-    <t>1 + 7.5 BAF</t>
-  </si>
-  <si>
-    <t>1 + 49 ORD</t>
-  </si>
-  <si>
-    <t>2 + 15 BAF</t>
-  </si>
-  <si>
-    <t>3 + 80 BAF</t>
-  </si>
-  <si>
-    <t>4 + 90 ORD</t>
-  </si>
-  <si>
-    <t>6 + 36 BAF</t>
-  </si>
-  <si>
-    <t>7 + 49.5 ORD</t>
-  </si>
-  <si>
-    <t>7 + 66 BAF</t>
-  </si>
-  <si>
-    <t>8 + 62 BAF</t>
-  </si>
-  <si>
-    <t>9 + 99 BAF</t>
-  </si>
-  <si>
-    <t>10 + 13 BAF</t>
-  </si>
-  <si>
-    <t>11 + 12 ORD</t>
-  </si>
-  <si>
-    <t>11 + 24 BAF</t>
-  </si>
-  <si>
-    <t>11 + 63 ORD</t>
-  </si>
-  <si>
-    <t>11 + 73 BAF</t>
-  </si>
-  <si>
-    <t>1 + 04</t>
-  </si>
-  <si>
-    <t>2 + 04</t>
-  </si>
-  <si>
-    <t>2 + 52</t>
-  </si>
-  <si>
-    <t>3 + 63</t>
-  </si>
-  <si>
-    <t>3 + 98</t>
-  </si>
-  <si>
-    <t>5 + 00</t>
-  </si>
-  <si>
-    <t>5 + 09</t>
-  </si>
-  <si>
-    <t>5 + 62</t>
-  </si>
-  <si>
-    <t>6 + 13</t>
-  </si>
-  <si>
-    <t>6 + 97</t>
-  </si>
-  <si>
-    <t>7 + 30</t>
-  </si>
-  <si>
-    <t>7 + 50</t>
-  </si>
-  <si>
-    <t>7 + 97</t>
-  </si>
-  <si>
-    <t>9 + 05</t>
-  </si>
-  <si>
-    <t>9 + 26</t>
-  </si>
-  <si>
-    <t>9 + 68</t>
-  </si>
-  <si>
-    <t>1 + 11.5 BAF</t>
-  </si>
-  <si>
-    <t>1 + 99 ORD</t>
-  </si>
-  <si>
-    <t>2 + 16 BAF</t>
-  </si>
-  <si>
-    <t>2 + 57</t>
-  </si>
-  <si>
-    <t>2 + 67</t>
-  </si>
-  <si>
-    <t>3 + 9 ORD</t>
-  </si>
-  <si>
-    <t>3 + 31</t>
-  </si>
-  <si>
-    <t>3 + 65 ORD</t>
-  </si>
-  <si>
-    <t>3 + 95.5 ORD</t>
-  </si>
-  <si>
-    <t>4 + 14.5</t>
-  </si>
-  <si>
-    <t>4 + 36</t>
-  </si>
-  <si>
-    <t>4 + 50</t>
-  </si>
-  <si>
-    <t>4 + 78 ORD</t>
-  </si>
-  <si>
-    <t>1 + 4</t>
-  </si>
-  <si>
-    <t>1 + 52</t>
-  </si>
-  <si>
-    <t>1 + 83</t>
-  </si>
-  <si>
-    <t>2 + 63</t>
-  </si>
-  <si>
-    <t>2 + 98</t>
-  </si>
-  <si>
-    <t>3 + 93</t>
-  </si>
-  <si>
-    <t>4 + 00</t>
-  </si>
-  <si>
-    <t>4 + 09</t>
-  </si>
-  <si>
-    <t>4 + 56</t>
-  </si>
-  <si>
-    <t>4 + 65</t>
-  </si>
-  <si>
-    <t>5 + 13</t>
-  </si>
-  <si>
-    <t>5 + 48</t>
-  </si>
-  <si>
-    <t>6 + 30</t>
-  </si>
-  <si>
-    <t>10 + 80</t>
-  </si>
-  <si>
-    <t>1 + 38 ORD</t>
-  </si>
-  <si>
-    <t>1 + 71 ORD</t>
-  </si>
-  <si>
-    <t>1 + 77 BAF</t>
-  </si>
-  <si>
     <t>Station</t>
   </si>
   <si>
@@ -332,13 +149,211 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Channel 21</t>
+  </si>
+  <si>
+    <t>Channel 19</t>
+  </si>
+  <si>
+    <t>Channel 12</t>
+  </si>
+  <si>
+    <t>Station 1 + 04</t>
+  </si>
+  <si>
+    <t>Station 1 + 52</t>
+  </si>
+  <si>
+    <t>Station 1 + 83</t>
+  </si>
+  <si>
+    <t>Station 2 + 63</t>
+  </si>
+  <si>
+    <t>Station 2 + 98</t>
+  </si>
+  <si>
+    <t>Station 3 + 93</t>
+  </si>
+  <si>
+    <t>Station 4 + 00</t>
+  </si>
+  <si>
+    <t>Station 4 + 09</t>
+  </si>
+  <si>
+    <t>Station 4 + 56</t>
+  </si>
+  <si>
+    <t>Station 4 + 65</t>
+  </si>
+  <si>
+    <t>Station 5 + 13</t>
+  </si>
+  <si>
+    <t>Station 5 + 48</t>
+  </si>
+  <si>
+    <t>Station 6 + 30</t>
+  </si>
+  <si>
+    <t>Station 6 + 93</t>
+  </si>
+  <si>
+    <t>Channel 13</t>
+  </si>
+  <si>
+    <t>Station 1 + 11.5 BAF</t>
+  </si>
+  <si>
+    <t>Station 1 + 38.5 ORD</t>
+  </si>
+  <si>
+    <t>Station 1 + 71 BAF</t>
+  </si>
+  <si>
+    <t>Station 1 + 77 ORD</t>
+  </si>
+  <si>
+    <t>Station 1 + 99 ORD</t>
+  </si>
+  <si>
+    <t>Station 2 + 16 BAF</t>
+  </si>
+  <si>
+    <t>Station 2 + 57 ORD</t>
+  </si>
+  <si>
+    <t>Station 2 + 67 BAF</t>
+  </si>
+  <si>
+    <t>Station 3 + 09 ORD</t>
+  </si>
+  <si>
+    <t>Station 3 + 31 BAF</t>
+  </si>
+  <si>
+    <t>Station 3 + 65 ORD</t>
+  </si>
+  <si>
+    <t>Station 3 + 95.5 ORD</t>
+  </si>
+  <si>
+    <t>Station 4 + 14.5 BAF</t>
+  </si>
+  <si>
+    <t>Station 4 + 36 ORD</t>
+  </si>
+  <si>
+    <t>Station 4 + 50 BAF</t>
+  </si>
+  <si>
+    <t>Station 4 + 78 ORD</t>
+  </si>
+  <si>
+    <t>Station 01 + 04</t>
+  </si>
+  <si>
+    <t>Station 02 + 04</t>
+  </si>
+  <si>
+    <t>Station 02 + 52</t>
+  </si>
+  <si>
+    <t>Station 03 + 63</t>
+  </si>
+  <si>
+    <t>Station 03 + 98</t>
+  </si>
+  <si>
+    <t>Station 05 + 00</t>
+  </si>
+  <si>
+    <t>Station 05 + 09</t>
+  </si>
+  <si>
+    <t>Station 05 + 62</t>
+  </si>
+  <si>
+    <t>Station 06 + 13</t>
+  </si>
+  <si>
+    <t>Station 06 + 97</t>
+  </si>
+  <si>
+    <t>Station 07 + 30</t>
+  </si>
+  <si>
+    <t>Station 07 + 50</t>
+  </si>
+  <si>
+    <t>Station 07 + 97</t>
+  </si>
+  <si>
+    <t>Station 09 + 05</t>
+  </si>
+  <si>
+    <t>Station 09 + 26</t>
+  </si>
+  <si>
+    <t>Station 09 + 68</t>
+  </si>
+  <si>
+    <t>Station 10 + 98</t>
+  </si>
+  <si>
+    <t>Station 01 + 07.5 BAF</t>
+  </si>
+  <si>
+    <t>Station 01 + 49 ORD</t>
+  </si>
+  <si>
+    <t>Station 02 + 15 BAF</t>
+  </si>
+  <si>
+    <t>Station 03 + 80 BAF</t>
+  </si>
+  <si>
+    <t>Station 04 + 90 ORD</t>
+  </si>
+  <si>
+    <t>Station 06 + 36 BAF</t>
+  </si>
+  <si>
+    <t>Station 07 + 49.5 ORD</t>
+  </si>
+  <si>
+    <t>Station 07 + 66 BAF</t>
+  </si>
+  <si>
+    <t>Station 08 + 62 BAF</t>
+  </si>
+  <si>
+    <t>Station 09 + 99 ORD</t>
+  </si>
+  <si>
+    <t>Station 10 + 13 BAF</t>
+  </si>
+  <si>
+    <t>Station 11 + 12 ORD</t>
+  </si>
+  <si>
+    <t>Station 11 + 24 BAF</t>
+  </si>
+  <si>
+    <t>Station 11 + 63 ORD</t>
+  </si>
+  <si>
+    <t>Station 11 + 73 BAF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,18 +379,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -862,12 +865,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="11.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.21875" style="3" customWidth="1"/>
     <col min="3" max="7" width="8.88671875" style="7"/>
   </cols>
@@ -877,25 +880,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -904,12 +907,12 @@
       <c r="O1" s="4"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>21</v>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C2" s="7">
         <v>4.4000000000000004</v>
@@ -932,11 +935,11 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>21</v>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="C3" s="7">
         <v>4.3499999999999996</v>
@@ -959,11 +962,11 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>21</v>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7">
         <v>6.51</v>
@@ -986,11 +989,11 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>21</v>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C5" s="7">
         <v>3.89</v>
@@ -1013,11 +1016,11 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>21</v>
+      <c r="A6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C6" s="7">
         <v>1.75</v>
@@ -1040,11 +1043,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>21</v>
+      <c r="A7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7">
         <v>5.92</v>
@@ -1066,12 +1069,12 @@
         <v>6.3920000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>21</v>
+    <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7">
         <v>4.16</v>
@@ -1094,11 +1097,11 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>21</v>
+      <c r="A9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7">
         <v>5.77</v>
@@ -1121,11 +1124,11 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>21</v>
+      <c r="A10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C10" s="7">
         <v>3.04</v>
@@ -1148,11 +1151,11 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>21</v>
+      <c r="A11" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C11" s="7">
         <v>2.3199999999999998</v>
@@ -1175,11 +1178,11 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>21</v>
+      <c r="A12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C12" s="7">
         <v>2.97</v>
@@ -1202,11 +1205,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>21</v>
+      <c r="A13" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C13" s="7">
         <v>4.9400000000000004</v>
@@ -1229,11 +1232,11 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>21</v>
+      <c r="A14" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="C14" s="7">
         <v>5.47</v>
@@ -1256,11 +1259,11 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>21</v>
+      <c r="A15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7">
         <v>3.68</v>
@@ -1283,11 +1286,11 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>21</v>
+      <c r="A16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C16" s="9">
         <v>5.88</v>
@@ -1310,11 +1313,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>19</v>
+      <c r="A17" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C17" s="7">
         <v>2.46</v>
@@ -1340,11 +1343,11 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>19</v>
+      <c r="A18" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C18" s="7">
         <v>5.65</v>
@@ -1369,11 +1372,11 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>19</v>
+      <c r="A19" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C19" s="7">
         <v>9.81</v>
@@ -1399,11 +1402,11 @@
       <c r="T19" s="7"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>19</v>
+      <c r="A20" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C20" s="7">
         <v>5.91</v>
@@ -1428,11 +1431,11 @@
       <c r="R20" s="7"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>19</v>
+      <c r="A21" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C21" s="7">
         <v>15.52</v>
@@ -1457,11 +1460,11 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>19</v>
+      <c r="A22" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C22" s="7">
         <v>5.34</v>
@@ -1486,11 +1489,11 @@
       <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>19</v>
+      <c r="A23" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7">
         <v>5.31</v>
@@ -1515,11 +1518,11 @@
       <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>19</v>
+      <c r="A24" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C24" s="7">
         <v>2.0099999999999998</v>
@@ -1544,11 +1547,11 @@
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>19</v>
+      <c r="A25" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C25" s="7">
         <v>1.78</v>
@@ -1573,11 +1576,11 @@
       <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>19</v>
+      <c r="A26" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C26" s="7">
         <v>5.05</v>
@@ -1602,11 +1605,11 @@
       <c r="R26" s="7"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>19</v>
+      <c r="A27" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C27" s="7">
         <v>8.66</v>
@@ -1631,11 +1634,11 @@
       <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>19</v>
+      <c r="A28" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C28" s="7">
         <v>7.72</v>
@@ -1660,11 +1663,11 @@
       <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>19</v>
+      <c r="A29" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C29" s="7">
         <v>2.1</v>
@@ -1689,11 +1692,11 @@
       <c r="R29" s="7"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>19</v>
+      <c r="A30" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7">
         <v>3.45</v>
@@ -1718,11 +1721,11 @@
       <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>19</v>
+      <c r="A31" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C31" s="7">
         <v>2.62</v>
@@ -1747,11 +1750,11 @@
       <c r="R31" s="7"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>19</v>
+      <c r="A32" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C32" s="7">
         <v>2.75</v>
@@ -1776,8 +1779,8 @@
       <c r="R32" s="7"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>19</v>
+      <c r="A33" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>58</v>
@@ -1805,11 +1808,11 @@
       <c r="R33" s="7"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>13</v>
+      <c r="A34" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C34" s="7">
         <v>1.28</v>
@@ -1834,11 +1837,11 @@
       <c r="R34" s="7"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>13</v>
+      <c r="A35" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C35" s="7">
         <v>1.56</v>
@@ -1863,11 +1866,11 @@
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>13</v>
+      <c r="A36" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C36" s="7">
         <v>0.71</v>
@@ -1893,11 +1896,11 @@
       <c r="T36" s="7"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>13</v>
+      <c r="A37" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -1922,11 +1925,11 @@
       <c r="R37" s="7"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>13</v>
+      <c r="A38" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C38" s="7">
         <v>0.99</v>
@@ -1951,11 +1954,11 @@
       <c r="R38" s="7"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>13</v>
+      <c r="A39" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C39" s="7">
         <v>0.97</v>
@@ -1980,11 +1983,11 @@
       <c r="R39" s="7"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>13</v>
+      <c r="A40" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40" s="7">
         <v>2.89</v>
@@ -2009,11 +2012,11 @@
       <c r="R40" s="7"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>13</v>
+      <c r="A41" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" s="7">
         <v>1.33</v>
@@ -2038,11 +2041,11 @@
       <c r="R41" s="7"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <v>13</v>
+      <c r="A42" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42" s="7">
         <v>1.1499999999999999</v>
@@ -2067,11 +2070,11 @@
       <c r="R42" s="7"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>13</v>
+      <c r="A43" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C43" s="7">
         <v>1.83</v>
@@ -2096,11 +2099,11 @@
       <c r="R43" s="7"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>13</v>
+      <c r="A44" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C44" s="7">
         <v>1.75</v>
@@ -2125,11 +2128,11 @@
       <c r="R44" s="7"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>13</v>
+      <c r="A45" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C45" s="7">
         <v>1.17</v>
@@ -2154,11 +2157,11 @@
       <c r="R45" s="7"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>13</v>
+      <c r="A46" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C46" s="7">
         <v>2.1800000000000002</v>
@@ -2183,11 +2186,11 @@
       <c r="R46" s="7"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>13</v>
+      <c r="A47" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C47" s="7">
         <v>1.6</v>
@@ -2212,11 +2215,11 @@
       <c r="R47" s="7"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>13</v>
+      <c r="A48" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C48" s="7">
         <v>2.19</v>
@@ -2241,11 +2244,11 @@
       <c r="R48" s="7"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>13</v>
+      <c r="A49" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C49" s="9">
         <v>1.74</v>
@@ -2270,11 +2273,11 @@
       <c r="R49" s="7"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>12</v>
+      <c r="A50" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C50" s="7">
         <v>2.95</v>
@@ -2297,11 +2300,11 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+      <c r="A51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C51" s="7">
         <v>4.82</v>
@@ -2324,11 +2327,11 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>12</v>
+      <c r="A52" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C52" s="7">
         <v>5.55</v>
@@ -2351,11 +2354,11 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>12</v>
+      <c r="A53" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C53" s="7">
         <v>1.4</v>
@@ -2378,11 +2381,11 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>12</v>
+      <c r="A54" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C54" s="7">
         <v>2.86</v>
@@ -2405,11 +2408,11 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>12</v>
+      <c r="A55" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C55" s="7">
         <v>9.08</v>
@@ -2432,11 +2435,11 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>12</v>
+      <c r="A56" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C56" s="7">
         <v>8.4</v>
@@ -2459,11 +2462,11 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>12</v>
+      <c r="A57" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C57" s="7">
         <v>5.58</v>
@@ -2486,11 +2489,11 @@
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>12</v>
+      <c r="A58" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C58" s="7">
         <v>2.5499999999999998</v>
@@ -2513,11 +2516,11 @@
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>12</v>
+      <c r="A59" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C59" s="7">
         <v>2.78</v>
@@ -2540,11 +2543,11 @@
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>12</v>
+      <c r="A60" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C60" s="7">
         <v>2.61</v>
@@ -2567,11 +2570,11 @@
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>12</v>
+      <c r="A61" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C61" s="7">
         <v>0.99</v>
@@ -2594,11 +2597,11 @@
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>12</v>
+      <c r="A62" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C62" s="7">
         <v>0.85</v>
@@ -2621,11 +2624,11 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>12</v>
+      <c r="A63" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" s="7">
         <v>4.51</v>

</xml_diff>